<commit_message>
feat: 10. binarySearch / problem1
</commit_message>
<xml_diff>
--- a/정리.xlsx
+++ b/정리.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KDJ\Desktop\algorithm-practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82313868-8CBE-4CE1-81BE-4B0C426E8990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1EC4F2-34FA-4955-AB57-3EC23B5139B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="855" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="목차" sheetId="1" r:id="rId1"/>
     <sheet name="temp" sheetId="3" r:id="rId2"/>
-    <sheet name="DFS,BFS" sheetId="32" r:id="rId3"/>
-    <sheet name="dynamicProgramming" sheetId="31" r:id="rId4"/>
-    <sheet name="greedy" sheetId="30" r:id="rId5"/>
-    <sheet name="bruteForce" sheetId="28" r:id="rId6"/>
-    <sheet name="sort" sheetId="26" r:id="rId7"/>
-    <sheet name="heap" sheetId="25" r:id="rId8"/>
-    <sheet name="stack-queue" sheetId="24" r:id="rId9"/>
-    <sheet name="hash" sheetId="23" r:id="rId10"/>
-    <sheet name="기타 팁" sheetId="27" r:id="rId11"/>
-    <sheet name="실수목록" sheetId="29" r:id="rId12"/>
-    <sheet name="커밋컨벤션" sheetId="19" r:id="rId13"/>
+    <sheet name="binarySearch" sheetId="33" r:id="rId3"/>
+    <sheet name="DFS,BFS" sheetId="32" r:id="rId4"/>
+    <sheet name="dynamicProgramming" sheetId="31" r:id="rId5"/>
+    <sheet name="greedy" sheetId="30" r:id="rId6"/>
+    <sheet name="bruteForce" sheetId="28" r:id="rId7"/>
+    <sheet name="sort" sheetId="26" r:id="rId8"/>
+    <sheet name="heap" sheetId="25" r:id="rId9"/>
+    <sheet name="stack-queue" sheetId="24" r:id="rId10"/>
+    <sheet name="hash" sheetId="23" r:id="rId11"/>
+    <sheet name="기타 팁" sheetId="27" r:id="rId12"/>
+    <sheet name="실수목록" sheetId="29" r:id="rId13"/>
+    <sheet name="커밋컨벤션" sheetId="19" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="464">
   <si>
     <t>NO</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3431,6 +3432,114 @@
   </si>
   <si>
     <t>따라서 visited를 잘 이용하도록 재귀적으로 잘 만들어주면 된다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>type cast</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>타입을 지정해줄 때 사용할 수 있는 방법은 두가지이다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>int number를 long long으로 cast해서 사용하고 싶을 때 다음과 같은 두 방법으로 사용할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C 스타일 방식</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(long long) number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C++ 스타일 방식</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>static_cast&lt;long long&gt; number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C++방식으로 하는 것이 더 명시적이고 타입 안정성이 높아서 C++에선 후자 추천</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>참조형 변수 가지는 함수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C에서는 참조형 변수를 가지는 함수를 만들 때 파라미터 선언에서 포인터를 주고</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>함수 내용에 포인터가 들어간 연산을 해야했음.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>하지만 C++에서는 파라미터에서 &amp;변수로 선언해서</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>그냥 변수처럼 연산하면 됨.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이분 탐색</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이분 탐색은 어떤 범위에 대해 특정 조건을 만족하는 답을 구할 때 사용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본적으로 함수의 사잇값 정리와 비슷한 내용임.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>로직에서 중요한 것은 left와 right의 중간을 mid로 설정하는데</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mid의 값에 따라 그 다음 범위를 좁혀야하는데 가능한 경우가 2가지 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>left = mid + 1 혹은 right = mid - 1로하기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>left = mid 혹은 right = mid로 하기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>로직에 맞게 범위를 설정해주면 된다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 입국 심사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>로직이나 아이디어에는 특별한 것은 없다. 이분 탐색의 기본</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>조심해야 할 것은 범위인데 나는 가장 오래걸릴 때를 생각해서 int최대를 넘어가는 것은 생각했다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>따라서 답을 long long으로 내는 것 까지는 생각해서 (실수해서 오래걸렸지만..) 해결했다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>하지만 실수하기 쉬운 것은 vector를 돌며 몫을 더해줄 때 이미 넘어버렸다면 거기서 return해버리는 것이다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>심사관들이 심사를 너무 잘해서 몫이 너무 커져서 overflow가 나는 경우이다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4013,7 +4122,7 @@
         <xdr:cNvPr id="2" name="직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60D1DBAA-8843-4650-842A-3DC33D4A4487}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ADA3D1B-2FE5-4C85-AC5A-2461A09075BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4084,6 +4193,77 @@
         <xdr:cNvPr id="2" name="직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60D1DBAA-8843-4650-842A-3DC33D4A4487}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5143500" y="914400"/>
+          <a:ext cx="2457450" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="50800">
+          <a:solidFill>
+            <a:srgbClr val="6495ED"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="직사각형 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54C8D657-6461-49E3-9A69-70B86DB5E0F7}"/>
             </a:ext>
           </a:extLst>
@@ -4135,7 +4315,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4358,6 +4538,77 @@
         <xdr:cNvPr id="2" name="직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D162E98-66D1-4730-A0B0-A1DBF2E669CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5143500" y="914400"/>
+          <a:ext cx="2457450" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="50800">
+          <a:solidFill>
+            <a:srgbClr val="6495ED"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="직사각형 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA02FD81-C6B1-4FCC-83C4-2DA397C06454}"/>
             </a:ext>
           </a:extLst>
@@ -4475,7 +4726,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4546,7 +4797,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5561,7 +5812,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5632,7 +5883,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5703,7 +5954,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5774,7 +6025,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5959,77 +6210,6 @@
             <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
             <a:t>.</a:t>
           </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="직사각형 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ADA3D1B-2FE5-4C85-AC5A-2461A09075BA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5143500" y="914400"/>
-          <a:ext cx="2457450" cy="723900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="50800">
-          <a:solidFill>
-            <a:srgbClr val="6495ED"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
           <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -6304,7 +6484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -6489,6 +6669,520 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27DC9AE-D3F3-4D99-93B4-7F898251C61F}">
+  <dimension ref="A1:X64"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="5.625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="50"/>
+      <c r="M2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="13"/>
+    </row>
+    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50"/>
+      <c r="H3" s="6"/>
+      <c r="M3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+    </row>
+    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50"/>
+      <c r="H4" s="6"/>
+      <c r="M4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="9" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="11" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="N31" s="48"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="T31" s="48"/>
+      <c r="U31" s="48"/>
+      <c r="V31" s="48"/>
+      <c r="W31" s="48"/>
+      <c r="X31" s="48"/>
+    </row>
+    <row r="32" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E32" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="F32" s="48"/>
+      <c r="G32" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="N32" s="48"/>
+      <c r="O32" s="48"/>
+      <c r="P32" s="48"/>
+      <c r="Q32" s="48"/>
+      <c r="R32" s="48"/>
+      <c r="S32" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="T32" s="48"/>
+      <c r="U32" s="48"/>
+      <c r="V32" s="48"/>
+      <c r="W32" s="48"/>
+      <c r="X32" s="48"/>
+    </row>
+    <row r="33" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="48"/>
+      <c r="O33" s="48"/>
+      <c r="P33" s="48"/>
+      <c r="Q33" s="48"/>
+      <c r="R33" s="48"/>
+      <c r="S33" s="48"/>
+      <c r="T33" s="48"/>
+      <c r="U33" s="48"/>
+      <c r="V33" s="48"/>
+      <c r="W33" s="48"/>
+      <c r="X33" s="48"/>
+    </row>
+    <row r="34" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="48"/>
+      <c r="N34" s="48"/>
+      <c r="O34" s="48"/>
+      <c r="P34" s="48"/>
+      <c r="Q34" s="48"/>
+      <c r="R34" s="48"/>
+      <c r="S34" s="48"/>
+      <c r="T34" s="48"/>
+      <c r="U34" s="48"/>
+      <c r="V34" s="48"/>
+      <c r="W34" s="48"/>
+      <c r="X34" s="48"/>
+    </row>
+    <row r="35" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="48"/>
+      <c r="O35" s="48"/>
+      <c r="P35" s="48"/>
+      <c r="Q35" s="48"/>
+      <c r="R35" s="48"/>
+      <c r="S35" s="48"/>
+      <c r="T35" s="48"/>
+      <c r="U35" s="48"/>
+      <c r="V35" s="48"/>
+      <c r="W35" s="48"/>
+      <c r="X35" s="48"/>
+    </row>
+    <row r="36" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" s="48"/>
+      <c r="G36" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="48"/>
+      <c r="L36" s="48"/>
+      <c r="M36" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="N36" s="48"/>
+      <c r="O36" s="48"/>
+      <c r="P36" s="48"/>
+      <c r="Q36" s="48"/>
+      <c r="R36" s="48"/>
+      <c r="S36" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="T36" s="48"/>
+      <c r="U36" s="48"/>
+      <c r="V36" s="48"/>
+      <c r="W36" s="48"/>
+      <c r="X36" s="48"/>
+    </row>
+    <row r="37" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="48"/>
+      <c r="O37" s="48"/>
+      <c r="P37" s="48"/>
+      <c r="Q37" s="48"/>
+      <c r="R37" s="48"/>
+      <c r="S37" s="48"/>
+      <c r="T37" s="48"/>
+      <c r="U37" s="48"/>
+      <c r="V37" s="48"/>
+      <c r="W37" s="48"/>
+      <c r="X37" s="48"/>
+    </row>
+    <row r="38" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
+      <c r="L38" s="48"/>
+      <c r="M38" s="48"/>
+      <c r="N38" s="48"/>
+      <c r="O38" s="48"/>
+      <c r="P38" s="48"/>
+      <c r="Q38" s="48"/>
+      <c r="R38" s="48"/>
+      <c r="S38" s="48"/>
+      <c r="T38" s="48"/>
+      <c r="U38" s="48"/>
+      <c r="V38" s="48"/>
+      <c r="W38" s="48"/>
+      <c r="X38" s="48"/>
+    </row>
+    <row r="39" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="48"/>
+      <c r="L39" s="48"/>
+      <c r="M39" s="48"/>
+      <c r="N39" s="48"/>
+      <c r="O39" s="48"/>
+      <c r="P39" s="48"/>
+      <c r="Q39" s="48"/>
+      <c r="R39" s="48"/>
+      <c r="S39" s="48"/>
+      <c r="T39" s="48"/>
+      <c r="U39" s="48"/>
+      <c r="V39" s="48"/>
+      <c r="W39" s="48"/>
+      <c r="X39" s="48"/>
+    </row>
+    <row r="41" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+    </row>
+    <row r="43" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="30"/>
+      <c r="E46" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="30"/>
+      <c r="E47" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="29"/>
+    </row>
+    <row r="52" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+    </row>
+    <row r="54" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D55" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+    </row>
+    <row r="59" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="27"/>
+    </row>
+    <row r="60" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D61" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D62" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D63" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D64" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A1:A7"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:L31"/>
+    <mergeCell ref="M31:R31"/>
+    <mergeCell ref="S31:X31"/>
+    <mergeCell ref="E36:F39"/>
+    <mergeCell ref="G32:L35"/>
+    <mergeCell ref="G36:L39"/>
+    <mergeCell ref="M32:R35"/>
+    <mergeCell ref="S32:X35"/>
+    <mergeCell ref="M36:R39"/>
+    <mergeCell ref="S36:X39"/>
+    <mergeCell ref="E32:F35"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1:A7" location="목차!A1" display="목차!A1" xr:uid="{77CFC214-F479-4364-A6C9-8FA33CBB468B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5CE60D-3F10-4903-B885-6CDA794FB40F}">
   <dimension ref="A1:Q94"/>
   <sheetViews>
@@ -6933,12 +7627,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8709AF78-8857-4867-B1DD-14A6DFC4B711}">
-  <dimension ref="A1:U71"/>
+  <dimension ref="A1:U87"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7285,19 +7979,19 @@
       </c>
       <c r="U64" s="42"/>
     </row>
-    <row r="65" spans="3:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N65" s="41" t="s">
         <v>104</v>
       </c>
       <c r="U65" s="42"/>
     </row>
-    <row r="66" spans="3:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N66" s="41" t="s">
         <v>384</v>
       </c>
       <c r="U66" s="42"/>
     </row>
-    <row r="67" spans="3:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N67" s="21"/>
       <c r="O67" s="38"/>
       <c r="P67" s="38"/>
@@ -7307,24 +8001,93 @@
       <c r="T67" s="38"/>
       <c r="U67" s="39"/>
     </row>
-    <row r="68" spans="3:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C68" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="69" spans="3:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69" s="3" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="70" spans="3:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="71" spans="3:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C71" s="3" t="s">
         <v>389</v>
+      </c>
+    </row>
+    <row r="73" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="13"/>
+    </row>
+    <row r="75" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="76" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="77" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D77" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="78" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D78" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="80" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C80" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="13"/>
+    </row>
+    <row r="84" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C84" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C85" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C86" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C87" s="3" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -7341,7 +8104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3223DD8B-A1C7-45C6-AA2E-038777BE51FF}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
@@ -7438,7 +8201,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53359E70-DA5A-4BCE-A940-CF5D8D1B11F9}">
   <dimension ref="A1:V125"/>
   <sheetViews>
@@ -8162,11 +8925,176 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA5DE37-041B-4789-BE71-8503090DF99E}">
+  <dimension ref="A1:Q59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="5.625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="50"/>
+      <c r="M2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="13"/>
+    </row>
+    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50"/>
+      <c r="H3" s="6"/>
+      <c r="M3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+    </row>
+    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50"/>
+      <c r="H4" s="6"/>
+      <c r="M4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="9" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="11" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="3" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="13"/>
+    </row>
+    <row r="30" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="14" t="s">
+        <v>458</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="32" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="3" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="3" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A7"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1:A7" location="목차!A1" display="목차!A1" xr:uid="{8677902B-B85D-4299-830A-AD50D626C60C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD41A1E1-188A-4F1E-BBC7-E090551937C4}">
   <dimension ref="A1:U118"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83:G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8676,7 +9604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900018B4-248B-4963-B8EF-D15D1FCEE962}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
@@ -8929,7 +9857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E7D2B5-3732-46A4-9814-CED24E1391C4}">
   <dimension ref="A1:U59"/>
   <sheetViews>
@@ -9225,7 +10153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFF7ADC-9B90-43D2-923E-01DE6568B968}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
@@ -9374,7 +10302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DCCDC4B-10B5-4FB8-B5BB-DE6FFA03CB16}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
@@ -9736,7 +10664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74305CAB-EF31-4180-A9B1-F3B919031D3D}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
@@ -10089,518 +11017,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27DC9AE-D3F3-4D99-93B4-7F898251C61F}">
-  <dimension ref="A1:X64"/>
-  <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="5.625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
-      <c r="M2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="13"/>
-    </row>
-    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="H3" s="6"/>
-      <c r="M3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-    </row>
-    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
-      <c r="H4" s="6"/>
-      <c r="M4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-    </row>
-    <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="9" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="11" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-    </row>
-    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E31" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="N31" s="48"/>
-      <c r="O31" s="48"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="48"/>
-      <c r="R31" s="48"/>
-      <c r="S31" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="T31" s="48"/>
-      <c r="U31" s="48"/>
-      <c r="V31" s="48"/>
-      <c r="W31" s="48"/>
-      <c r="X31" s="48"/>
-    </row>
-    <row r="32" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E32" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="F32" s="48"/>
-      <c r="G32" s="51" t="s">
-        <v>132</v>
-      </c>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="N32" s="48"/>
-      <c r="O32" s="48"/>
-      <c r="P32" s="48"/>
-      <c r="Q32" s="48"/>
-      <c r="R32" s="48"/>
-      <c r="S32" s="51" t="s">
-        <v>136</v>
-      </c>
-      <c r="T32" s="48"/>
-      <c r="U32" s="48"/>
-      <c r="V32" s="48"/>
-      <c r="W32" s="48"/>
-      <c r="X32" s="48"/>
-    </row>
-    <row r="33" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
-      <c r="M33" s="48"/>
-      <c r="N33" s="48"/>
-      <c r="O33" s="48"/>
-      <c r="P33" s="48"/>
-      <c r="Q33" s="48"/>
-      <c r="R33" s="48"/>
-      <c r="S33" s="48"/>
-      <c r="T33" s="48"/>
-      <c r="U33" s="48"/>
-      <c r="V33" s="48"/>
-      <c r="W33" s="48"/>
-      <c r="X33" s="48"/>
-    </row>
-    <row r="34" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="O34" s="48"/>
-      <c r="P34" s="48"/>
-      <c r="Q34" s="48"/>
-      <c r="R34" s="48"/>
-      <c r="S34" s="48"/>
-      <c r="T34" s="48"/>
-      <c r="U34" s="48"/>
-      <c r="V34" s="48"/>
-      <c r="W34" s="48"/>
-      <c r="X34" s="48"/>
-    </row>
-    <row r="35" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="48"/>
-      <c r="O35" s="48"/>
-      <c r="P35" s="48"/>
-      <c r="Q35" s="48"/>
-      <c r="R35" s="48"/>
-      <c r="S35" s="48"/>
-      <c r="T35" s="48"/>
-      <c r="U35" s="48"/>
-      <c r="V35" s="48"/>
-      <c r="W35" s="48"/>
-      <c r="X35" s="48"/>
-    </row>
-    <row r="36" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="F36" s="48"/>
-      <c r="G36" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="N36" s="48"/>
-      <c r="O36" s="48"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="48"/>
-      <c r="R36" s="48"/>
-      <c r="S36" s="51" t="s">
-        <v>137</v>
-      </c>
-      <c r="T36" s="48"/>
-      <c r="U36" s="48"/>
-      <c r="V36" s="48"/>
-      <c r="W36" s="48"/>
-      <c r="X36" s="48"/>
-    </row>
-    <row r="37" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
-      <c r="M37" s="48"/>
-      <c r="N37" s="48"/>
-      <c r="O37" s="48"/>
-      <c r="P37" s="48"/>
-      <c r="Q37" s="48"/>
-      <c r="R37" s="48"/>
-      <c r="S37" s="48"/>
-      <c r="T37" s="48"/>
-      <c r="U37" s="48"/>
-      <c r="V37" s="48"/>
-      <c r="W37" s="48"/>
-      <c r="X37" s="48"/>
-    </row>
-    <row r="38" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="48"/>
-      <c r="O38" s="48"/>
-      <c r="P38" s="48"/>
-      <c r="Q38" s="48"/>
-      <c r="R38" s="48"/>
-      <c r="S38" s="48"/>
-      <c r="T38" s="48"/>
-      <c r="U38" s="48"/>
-      <c r="V38" s="48"/>
-      <c r="W38" s="48"/>
-      <c r="X38" s="48"/>
-    </row>
-    <row r="39" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="48"/>
-      <c r="M39" s="48"/>
-      <c r="N39" s="48"/>
-      <c r="O39" s="48"/>
-      <c r="P39" s="48"/>
-      <c r="Q39" s="48"/>
-      <c r="R39" s="48"/>
-      <c r="S39" s="48"/>
-      <c r="T39" s="48"/>
-      <c r="U39" s="48"/>
-      <c r="V39" s="48"/>
-      <c r="W39" s="48"/>
-      <c r="X39" s="48"/>
-    </row>
-    <row r="41" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-    </row>
-    <row r="43" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="44" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="30" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="46" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="30"/>
-      <c r="E46" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="30"/>
-      <c r="E47" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="48" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="13"/>
-    </row>
-    <row r="51" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F51" s="29"/>
-    </row>
-    <row r="52" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-    </row>
-    <row r="54" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-    </row>
-    <row r="59" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="27"/>
-    </row>
-    <row r="60" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D61" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A1:A7"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:L31"/>
-    <mergeCell ref="M31:R31"/>
-    <mergeCell ref="S31:X31"/>
-    <mergeCell ref="E36:F39"/>
-    <mergeCell ref="G32:L35"/>
-    <mergeCell ref="G36:L39"/>
-    <mergeCell ref="M32:R35"/>
-    <mergeCell ref="S32:X35"/>
-    <mergeCell ref="M36:R39"/>
-    <mergeCell ref="S36:X39"/>
-    <mergeCell ref="E32:F35"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A1:A7" location="목차!A1" display="목차!A1" xr:uid="{77CFC214-F479-4364-A6C9-8FA33CBB468B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>